<commit_message>
Alterei alguns use cases
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/AdicionarStock.xlsx
+++ b/Modelos UML/Descrição UseCases/AdicionarStock.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\UseCase\Descrição UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Luís\3º ano\1º Semestre\DSS\Trabalho\DSS\Modelos UML\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC6D30D-A865-4799-AD93-9ED95871ACA2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Actor input</t>
   </si>
@@ -74,22 +73,28 @@
     <t>3. Apresenta o ecrã de adição de stock</t>
   </si>
   <si>
-    <t xml:space="preserve">4.1. Apresenta mensagem "Stock Inválido" </t>
-  </si>
-  <si>
     <t>4. Adiciona Stock de uma peça</t>
   </si>
   <si>
-    <t>5. Regista adição do stock</t>
-  </si>
-  <si>
-    <t>6. Indica que a adição  foi feita com sucesso</t>
+    <t>5. Verifica adição de stock</t>
+  </si>
+  <si>
+    <t>6. Regista adição do stock</t>
+  </si>
+  <si>
+    <t>7. Indica que a adição  foi feita com sucesso</t>
+  </si>
+  <si>
+    <t>4.1. Apresenta mensagem "Stock Inválido"</t>
+  </si>
+  <si>
+    <t>4.1 Dados da peça inválidos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -270,6 +275,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -281,18 +298,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,11 +612,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -627,40 +632,40 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -671,69 +676,78 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="13"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="14"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="14"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="14"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="3"/>
       <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="12"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="2" t="s">
+    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="12"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="13" t="s">
+    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="14"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="12"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="B6:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Descrição de use cases revisto
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/AdicionarStock.xlsx
+++ b/Modelos UML/Descrição UseCases/AdicionarStock.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\Luís\3º ano\1º Semestre\DSS\Trabalho\DSS\Modelos UML\Descrição UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\Modelos UML\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75A8EC8-413C-472B-9DAB-D7F68292E029}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,10 +58,6 @@
     <t>Lista de Stock foi alterada</t>
   </si>
   <si>
-    <t>Exceção 
-(Stock Inválido)</t>
-  </si>
-  <si>
     <t>Funcionário</t>
   </si>
   <si>
@@ -89,12 +86,16 @@
   </si>
   <si>
     <t>4.1 Dados da peça inválidos</t>
+  </si>
+  <si>
+    <t>Exceção 1
+[Stock Inválido] (Passo 4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -612,11 +613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -642,7 +643,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="14"/>
     </row>
@@ -679,13 +680,13 @@
       <c r="B7" s="11"/>
       <c r="C7" s="9"/>
       <c r="D7" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -693,13 +694,13 @@
       <c r="B9" s="12"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="12"/>
       <c r="C10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -707,37 +708,37 @@
       <c r="B11" s="12"/>
       <c r="C11" s="3"/>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12"/>
       <c r="C12" s="3"/>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12"/>
       <c r="C13" s="4"/>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="11" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="12"/>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionar Stock alterado e Packages
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/AdicionarStock.xlsx
+++ b/Modelos UML/Descrição UseCases/AdicionarStock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\Modelos UML\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75A8EC8-413C-472B-9DAB-D7F68292E029}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892CBF5D-94C1-4B8A-94B2-B51C72235C11}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Actor input</t>
   </si>
@@ -76,12 +76,6 @@
     <t>5. Verifica adição de stock</t>
   </si>
   <si>
-    <t>6. Regista adição do stock</t>
-  </si>
-  <si>
-    <t>7. Indica que a adição  foi feita com sucesso</t>
-  </si>
-  <si>
     <t>4.1. Apresenta mensagem "Stock Inválido"</t>
   </si>
   <si>
@@ -90,6 +84,15 @@
   <si>
     <t>Exceção 1
 [Stock Inválido] (Passo 4)</t>
+  </si>
+  <si>
+    <t>6. Adiciona peça a carros que precisem da mesma</t>
+  </si>
+  <si>
+    <t>7. Regista adição do stock</t>
+  </si>
+  <si>
+    <t>8. Indica que a adição  foi feita com sucesso</t>
   </si>
 </sst>
 </file>
@@ -614,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D15"/>
+  <dimension ref="B1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -715,40 +718,47 @@
       <c r="B12" s="12"/>
       <c r="C12" s="3"/>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="12"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="12"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="2" t="s">
-        <v>18</v>
+    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="12"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B15:B16"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B6:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correção de alguns promenores nos diagramas uml
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/AdicionarStock.xlsx
+++ b/Modelos UML/Descrição UseCases/AdicionarStock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\Modelos UML\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892CBF5D-94C1-4B8A-94B2-B51C72235C11}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72331A1C-7926-450C-A097-70B296B19AE0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Actor input</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Adicionar Stock</t>
   </si>
   <si>
-    <t>Lista de Stock foi alterada</t>
-  </si>
-  <si>
     <t>Funcionário</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
   </si>
   <si>
     <t>5. Verifica adição de stock</t>
-  </si>
-  <si>
-    <t>4.1. Apresenta mensagem "Stock Inválido"</t>
   </si>
   <si>
     <t>4.1 Dados da peça inválidos</t>
@@ -86,13 +80,16 @@
 [Stock Inválido] (Passo 4)</t>
   </si>
   <si>
-    <t>6. Adiciona peça a carros que precisem da mesma</t>
-  </si>
-  <si>
-    <t>7. Regista adição do stock</t>
-  </si>
-  <si>
-    <t>8. Indica que a adição  foi feita com sucesso</t>
+    <t>Stock de uma peça foi alterada</t>
+  </si>
+  <si>
+    <t>4.1. Apresenta mensagem "Peça Inválida"</t>
+  </si>
+  <si>
+    <t>6. Adiciona Stock e adiciona peça a carros que precisem da mesma</t>
+  </si>
+  <si>
+    <t>7. Indica que a adição  foi feita com sucesso</t>
   </si>
 </sst>
 </file>
@@ -617,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D16"/>
+  <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -628,7 +625,7 @@
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="20.75" customWidth="1"/>
     <col min="3" max="3" width="44.25" customWidth="1"/>
-    <col min="4" max="4" width="50.875" customWidth="1"/>
+    <col min="4" max="4" width="64.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -646,7 +643,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="14"/>
     </row>
@@ -664,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D5" s="16"/>
     </row>
@@ -683,13 +680,13 @@
       <c r="B7" s="11"/>
       <c r="C7" s="9"/>
       <c r="D7" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -697,13 +694,13 @@
       <c r="B9" s="12"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="12"/>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -711,7 +708,7 @@
       <c r="B11" s="12"/>
       <c r="C11" s="3"/>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -723,42 +720,35 @@
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="12"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="2" t="s">
-        <v>21</v>
+      <c r="B14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="12"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="B6:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>